<commit_message>
support visible character length for each column if there is length attribute in configuration.
</commit_message>
<xml_diff>
--- a/excel/template.xlsx
+++ b/excel/template.xlsx
@@ -178,125 +178,133 @@
   <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <protection locked="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <protection locked="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <protection locked="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true">
+      <alignment horizontal="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
       <protection locked="true"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment horizontal="right"/>
+      <alignment wrapText="true" horizontal="right"/>
       <protection locked="true"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment horizontal="right"/>
-      <protection locked="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="right"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
       <protection locked="true"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment horizontal="center"/>
+      <alignment wrapText="true" horizontal="center"/>
       <protection locked="true"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment horizontal="center"/>
-      <protection locked="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
       <protection locked="true"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <alignment horizontal="center"/>
-      <protection locked="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
-      <protection locked="true"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
+      <protection locked="true"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment wrapText="true"/>
       <protection locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -458,18 +466,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" hidden="true" width="21.66015625" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="35.6015625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="17.984375" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="14.9296875" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="19.66796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" hidden="true" width="4.0" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="14.0" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="14.0" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="12.0" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.0" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="6.0625" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="12.0" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="12.97265625" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="24.953125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="6.0625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.0546875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="28.91015625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="89.015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.66015625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="16.0" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="10.0" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="12.0" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="44.0" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
Fix bigInteger and bigdecimal
</commit_message>
<xml_diff>
--- a/excel/template.xlsx
+++ b/excel/template.xlsx
@@ -417,17 +417,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" hidden="true" width="20.02734375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.02734375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" hidden="true" width="16.6875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="16.6875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="44.0" customWidth="true"/>
-    <col min="4" max="4" width="25.94140625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="11.51953125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.9609375" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="18.72265625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="10.015625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="17.62890625" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="11.81640625" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="13.8203125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="21.6171875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="9.59765625" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="5.2578125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="15.6015625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="9.7578125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="14.6875" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="9.84765625" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="11.515625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="44.0" customWidth="true"/>
   </cols>
   <sheetData>

</xml_diff>